<commit_message>
Apply ACT_EFF=0 for DC cooling electricity (accounted for through VDA_FLOP)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SRV_DC_EH.xlsx
+++ b/SuppXLS/Scen_SRV_DC_EH.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62AA1F3-8572-438B-8810-1151CD99FB14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382E190B-B0AF-46D9-A29F-F03EBAB5B4C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="15390" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TOPINS" sheetId="2" r:id="rId1"/>
+    <sheet name="integration" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -26,17 +26,26 @@
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>SRVHET-DC-LT</t>
   </si>
@@ -81,6 +90,15 @@
   </si>
   <si>
     <t>IN</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>ACT_EFF</t>
+  </si>
+  <si>
+    <t>Other_Indexes</t>
   </si>
 </sst>
 </file>
@@ -419,26 +437,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D56313-9683-4DCD-B006-F6F3107A5280}">
-  <dimension ref="B3:I7"/>
+  <dimension ref="B3:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="9.06640625" style="1"/>
-    <col min="8" max="8" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -464,12 +484,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
+      <c r="G5" s="1" t="str">
+        <f t="shared" ref="G5:G7" si="0">F5</f>
+        <v>OUT</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>12</v>
@@ -478,12 +499,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>IN</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>13</v>
@@ -492,18 +514,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>2</v>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>OUT</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f>F11</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make combined electricity consumption of DCs on ANNUAL level equal to the end-use demand of DCs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SRV_DC_EH.xlsx
+++ b/SuppXLS/Scen_SRV_DC_EH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382E190B-B0AF-46D9-A29F-F03EBAB5B4C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CC6AF1-9627-4C96-B14A-8C6421C32801}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="integration" sheetId="2" r:id="rId1"/>
@@ -44,8 +44,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2070D2EC-AEEF-42E5-8008-CFEA22FBD9E3}</author>
+  </authors>
+  <commentList>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{2070D2EC-AEEF-42E5-8008-CFEA22FBD9E3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    lower consumption electricity that is not used for cooling. I.e. el for cooling + el for IT ca. = dc end-use demand</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>SRVHET-DC-LT</t>
   </si>
@@ -99,6 +117,12 @@
   </si>
   <si>
     <t>Other_Indexes</t>
+  </si>
+  <si>
+    <t>~TFM_UPD</t>
+  </si>
+  <si>
+    <t>EFF</t>
   </si>
 </sst>
 </file>
@@ -172,6 +196,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Balyk, Olexandr" id="{350715B6-622E-4E35-B498-CB0D8CC3C58C}" userId="Balyk, Olexandr" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -435,12 +465,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F15" dT="2021-04-21T11:38:55.94" personId="{350715B6-622E-4E35-B498-CB0D8CC3C58C}" id="{2070D2EC-AEEF-42E5-8008-CFEA22FBD9E3}">
+    <text>lower consumption electricity that is not used for cooling. I.e. el for cooling + el for IT ca. = dc end-use demand</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D56313-9683-4DCD-B006-F6F3107A5280}">
-  <dimension ref="B3:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D56313-9683-4DCD-B006-F6F3107A5280}">
+  <dimension ref="B3:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -578,7 +616,54 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.073</v>
+      </c>
+      <c r="G15" s="1">
+        <f>F15</f>
+        <v>1.073</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>